<commit_message>
DB tables with datatypes
</commit_message>
<xml_diff>
--- a/diagrams/online examinaton system/tables_1.xlsx
+++ b/diagrams/online examinaton system/tables_1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB71928-AE96-4FA5-AADA-FB9AA19E8834}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70799EE-21E3-4289-B765-2647AE5B4957}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="150">
   <si>
     <t xml:space="preserve">USER_PROFILE </t>
   </si>
@@ -678,7 +678,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
@@ -689,28 +689,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
@@ -719,6 +716,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1006,7 +1007,7 @@
   <dimension ref="A1:K87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,23 +1026,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="6"/>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="G1" s="10" t="s">
+      <c r="E1" s="12"/>
+      <c r="G1" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="J1" s="17" t="s">
+      <c r="H1" s="12"/>
+      <c r="J1" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="K1" s="17"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1188,14 +1189,14 @@
       <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="J8" s="10" t="s">
+      <c r="E8" s="19"/>
+      <c r="J8" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="K8" s="10"/>
+      <c r="K8" s="12"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -1230,10 +1231,10 @@
       <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="10"/>
+      <c r="H10" s="12"/>
       <c r="J10" s="3" t="s">
         <v>80</v>
       </c>
@@ -1326,12 +1327,8 @@
       <c r="H14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -1340,16 +1337,12 @@
       <c r="B15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="J15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="E15" s="12"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1378,10 +1371,10 @@
       <c r="E17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="10"/>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -1444,10 +1437,10 @@
       <c r="B21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="12"/>
+      <c r="E21" s="14"/>
       <c r="G21" s="3" t="s">
         <v>43</v>
       </c>
@@ -1516,16 +1509,16 @@
       <c r="E25" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G25" s="18" t="s">
+      <c r="G25" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="H25" s="19"/>
+      <c r="H25" s="18"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="10"/>
+      <c r="B26" s="12"/>
       <c r="G26" s="3" t="s">
         <v>1</v>
       </c>
@@ -1540,10 +1533,10 @@
       <c r="B27" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E27" s="12"/>
+      <c r="E27" s="14"/>
       <c r="G27" s="3" t="s">
         <v>68</v>
       </c>
@@ -1706,14 +1699,14 @@
       <c r="B36" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="E36" s="12"/>
-      <c r="G36" s="10" t="s">
+      <c r="E36" s="14"/>
+      <c r="G36" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="H36" s="10"/>
+      <c r="H36" s="12"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
@@ -1750,10 +1743,10 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="10"/>
+      <c r="B39" s="12"/>
       <c r="D39" s="4" t="s">
         <v>142</v>
       </c>
@@ -1808,10 +1801,10 @@
       <c r="B42" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G42" s="10" t="s">
+      <c r="G42" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="H42" s="10"/>
+      <c r="H42" s="12"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
@@ -1820,10 +1813,10 @@
       <c r="B43" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="E43" s="12"/>
+      <c r="E43" s="14"/>
       <c r="G43" s="3" t="s">
         <v>1</v>
       </c>
@@ -1900,10 +1893,10 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B48" s="10"/>
+      <c r="B48" s="12"/>
       <c r="G48" s="3" t="s">
         <v>35</v>
       </c>
@@ -1918,10 +1911,10 @@
       <c r="B49" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="D49" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="E49" s="10"/>
+      <c r="E49" s="12"/>
       <c r="G49" s="3" t="s">
         <v>36</v>
       </c>
@@ -1956,10 +1949,10 @@
       <c r="E51" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G51" s="11" t="s">
+      <c r="G51" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="H51" s="12"/>
+      <c r="H51" s="14"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
@@ -1982,10 +1975,10 @@
       <c r="B53" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D53" s="11" t="s">
+      <c r="D53" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="E53" s="12"/>
+      <c r="E53" s="14"/>
       <c r="G53" s="3" t="s">
         <v>132</v>
       </c>
@@ -2020,10 +2013,10 @@
       <c r="E55" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G55" s="11" t="s">
+      <c r="G55" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="H55" s="12"/>
+      <c r="H55" s="14"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
@@ -2086,10 +2079,10 @@
       <c r="B59" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D59" s="11" t="s">
+      <c r="D59" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="E59" s="12"/>
+      <c r="E59" s="14"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
@@ -2104,14 +2097,14 @@
       <c r="E60" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G60" s="16" t="s">
+      <c r="G60" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="H60" s="12"/>
-      <c r="I60" s="14" t="s">
+      <c r="H60" s="14"/>
+      <c r="I60" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="J60" s="15"/>
+      <c r="J60" s="11"/>
       <c r="K60" s="1"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -2129,10 +2122,10 @@
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="10" t="s">
+      <c r="A62" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="B62" s="10"/>
+      <c r="B62" s="12"/>
       <c r="D62" s="3" t="s">
         <v>112</v>
       </c>
@@ -2248,10 +2241,10 @@
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="10" t="s">
+      <c r="A72" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B72" s="10"/>
+      <c r="B72" s="12"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
@@ -2375,6 +2368,22 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D15:E15"/>
     <mergeCell ref="I60:J60"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="G1:H1"/>
@@ -2387,22 +2396,6 @@
     <mergeCell ref="G55:H55"/>
     <mergeCell ref="G51:H51"/>
     <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D59:E59"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
db tables with data type
</commit_message>
<xml_diff>
--- a/diagrams/online examinaton system/tables_1.xlsx
+++ b/diagrams/online examinaton system/tables_1.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70799EE-21E3-4289-B765-2647AE5B4957}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -151,13 +150,7 @@
     <t>TINY INT</t>
   </si>
   <si>
-    <t>STUDENT_CATEGORY_ID</t>
-  </si>
-  <si>
     <t>CHAR</t>
-  </si>
-  <si>
-    <t>STUDENT_CATEGORY_NAME</t>
   </si>
   <si>
     <t>EMP_CATEGORY</t>
@@ -495,12 +488,18 @@
   <si>
     <t>COURSE_TYPE(modular / tbc / crt)</t>
   </si>
+  <si>
+    <t>CLIENT_CATEGORY_ID</t>
+  </si>
+  <si>
+    <t>CLIENT_CATEGORY_NAME</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -689,6 +688,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -719,7 +719,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -784,7 +783,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -819,7 +818,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -996,55 +995,55 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="G18" sqref="G18:H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="1" max="1" width="33.5546875" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="13"/>
       <c r="C1" s="6"/>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="G1" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="H1" s="12"/>
-      <c r="J1" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="K1" s="15"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E1" s="13"/>
+      <c r="G1" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="13"/>
+      <c r="J1" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="K1" s="16"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1064,13 +1063,13 @@
         <v>2</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1084,19 +1083,19 @@
         <v>7</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1110,19 +1109,19 @@
         <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1136,10 +1135,10 @@
         <v>37</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>35</v>
@@ -1148,7 +1147,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1168,7 +1167,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1182,23 +1181,23 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="J8" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="K8" s="12"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D8" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="E8" s="20"/>
+      <c r="J8" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K8" s="13"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1212,13 +1211,13 @@
         <v>38</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -1231,18 +1230,18 @@
       <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" s="12"/>
+      <c r="G10" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="13"/>
       <c r="J10" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -1262,13 +1261,13 @@
         <v>2</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -1282,7 +1281,7 @@
         <v>37</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>29</v>
@@ -1294,7 +1293,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="3" t="s">
         <v>20</v>
       </c>
@@ -1314,7 +1313,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="3" t="s">
         <v>22</v>
       </c>
@@ -1327,24 +1326,24 @@
       <c r="H14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="E15" s="12"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D15" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
@@ -1352,13 +1351,13 @@
         <v>27</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
@@ -1366,17 +1365,17 @@
         <v>29</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>45</v>
+        <v>149</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="H17" s="12"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G17" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="13"/>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
@@ -1396,7 +1395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
@@ -1410,13 +1409,13 @@
         <v>37</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
@@ -1424,31 +1423,31 @@
         <v>4</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="14"/>
+      <c r="D21" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="15"/>
       <c r="G21" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
         <v>34</v>
       </c>
@@ -1456,10 +1455,10 @@
         <v>18</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>35</v>
@@ -1468,7 +1467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="3" t="s">
         <v>35</v>
       </c>
@@ -1476,7 +1475,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>4</v>
@@ -1488,7 +1487,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="3" t="s">
         <v>36</v>
       </c>
@@ -1502,23 +1501,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="D25" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G25" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="H25" s="18"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="12"/>
+      <c r="G25" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="H25" s="19"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="13"/>
       <c r="G26" s="3" t="s">
         <v>1</v>
       </c>
@@ -1526,130 +1525,130 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E27" s="14"/>
+      <c r="D27" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="15"/>
       <c r="G27" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G29" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H30" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>35</v>
@@ -1664,9 +1663,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>4</v>
@@ -1684,31 +1683,31 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E36" s="14"/>
-      <c r="G36" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="H36" s="12"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D36" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" s="15"/>
+      <c r="G36" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="H36" s="13"/>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
@@ -1716,21 +1715,21 @@
         <v>37</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="D38" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>9</v>
@@ -1739,16 +1738,16 @@
         <v>41</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B39" s="12"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="13"/>
       <c r="D39" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>18</v>
@@ -1760,9 +1759,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>2</v>
@@ -1780,9 +1779,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>2</v>
@@ -1794,29 +1793,29 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="H42" s="13"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G42" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="H42" s="12"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D43" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="E43" s="14"/>
+      <c r="D43" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E43" s="15"/>
       <c r="G43" s="3" t="s">
         <v>1</v>
       </c>
@@ -1824,7 +1823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="3" t="s">
         <v>35</v>
       </c>
@@ -1832,19 +1831,19 @@
         <v>2</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="3" t="s">
         <v>36</v>
       </c>
@@ -1852,19 +1851,19 @@
         <v>37</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>27</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="D46" s="3" t="s">
         <v>35</v>
       </c>
@@ -1872,13 +1871,13 @@
         <v>2</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="D47" s="3" t="s">
         <v>36</v>
       </c>
@@ -1886,17 +1885,17 @@
         <v>37</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B48" s="12"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="13"/>
       <c r="G48" s="3" t="s">
         <v>35</v>
       </c>
@@ -1904,17 +1903,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11">
       <c r="A49" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D49" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="E49" s="12"/>
+      <c r="D49" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E49" s="13"/>
       <c r="G49" s="3" t="s">
         <v>36</v>
       </c>
@@ -1922,108 +1921,108 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11">
       <c r="A50" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11">
       <c r="A51" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G51" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="H51" s="14"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G51" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="H51" s="15"/>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G52" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="E53" s="15"/>
+      <c r="G53" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H53" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="H52" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D53" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="E53" s="14"/>
-      <c r="G53" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11">
       <c r="A55" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G55" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="H55" s="14"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G55" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="H55" s="15"/>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>35</v>
@@ -2032,18 +2031,18 @@
         <v>2</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>36</v>
@@ -2052,39 +2051,39 @@
         <v>37</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D59" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="E59" s="14"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D59" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="E59" s="15"/>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60" s="3" t="s">
         <v>36</v>
       </c>
@@ -2092,74 +2091,74 @@
         <v>37</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G60" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="H60" s="14"/>
-      <c r="I60" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="J60" s="11"/>
+      <c r="G60" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="H60" s="15"/>
+      <c r="I60" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="J60" s="12"/>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11">
       <c r="D61" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H61" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E61" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H61" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B62" s="12"/>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B62" s="13"/>
       <c r="D62" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11">
       <c r="A63" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H63" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11">
       <c r="A64" s="3" t="s">
         <v>1</v>
       </c>
@@ -2173,15 +2172,15 @@
         <v>2</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H64" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>9</v>
@@ -2193,37 +2192,37 @@
         <v>37</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H65" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="3" t="s">
         <v>35</v>
       </c>
@@ -2232,7 +2231,7 @@
       </c>
       <c r="J69" s="8"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="3" t="s">
         <v>36</v>
       </c>
@@ -2240,117 +2239,117 @@
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="B72" s="12"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
+      <c r="A72" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B72" s="13"/>
+    </row>
+    <row r="73" spans="1:10">
       <c r="A73" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
       <c r="A74" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
       <c r="A75" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B76" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="B78" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B77" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+      <c r="B79" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B80" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B78" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:2">
       <c r="A81" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2">
       <c r="A82" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B82" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:2">
       <c r="A83" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
       <c r="A84" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2">
       <c r="A85" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
       <c r="A86" s="3" t="s">
         <v>35</v>
       </c>
@@ -2358,7 +2357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2">
       <c r="A87" s="3" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
DB tables with data types
</commit_message>
<xml_diff>
--- a/diagrams/online examinaton system/tables_1.xlsx
+++ b/diagrams/online examinaton system/tables_1.xlsx
@@ -689,34 +689,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -995,7 +995,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1025,23 +1025,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="11"/>
       <c r="C1" s="6"/>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="G1" s="13" t="s">
+      <c r="E1" s="11"/>
+      <c r="G1" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="J1" s="16" t="s">
+      <c r="H1" s="11"/>
+      <c r="J1" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="K1" s="16"/>
+      <c r="K1" s="18"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="3" t="s">
@@ -1188,14 +1188,14 @@
       <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="J8" s="13" t="s">
+      <c r="E8" s="14"/>
+      <c r="J8" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="K8" s="13"/>
+      <c r="K8" s="11"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
@@ -1230,10 +1230,10 @@
       <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="13"/>
+      <c r="H10" s="11"/>
       <c r="J10" s="3" t="s">
         <v>78</v>
       </c>
@@ -1336,10 +1336,10 @@
       <c r="B15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="E15" s="13"/>
+      <c r="E15" s="11"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
     </row>
@@ -1370,10 +1370,10 @@
       <c r="E17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="13"/>
+      <c r="H17" s="11"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
@@ -1436,10 +1436,10 @@
       <c r="B21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="15"/>
+      <c r="E21" s="13"/>
       <c r="G21" s="3" t="s">
         <v>148</v>
       </c>
@@ -1508,16 +1508,16 @@
       <c r="E25" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G25" s="18" t="s">
+      <c r="G25" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="H25" s="19"/>
+      <c r="H25" s="20"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="13"/>
+      <c r="B26" s="11"/>
       <c r="G26" s="3" t="s">
         <v>1</v>
       </c>
@@ -1532,10 +1532,10 @@
       <c r="B27" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="E27" s="15"/>
+      <c r="E27" s="13"/>
       <c r="G27" s="3" t="s">
         <v>66</v>
       </c>
@@ -1698,14 +1698,14 @@
       <c r="B36" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D36" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E36" s="15"/>
-      <c r="G36" s="13" t="s">
+      <c r="E36" s="13"/>
+      <c r="G36" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="H36" s="13"/>
+      <c r="H36" s="11"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="3" t="s">
@@ -1742,10 +1742,10 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B39" s="13"/>
+      <c r="B39" s="11"/>
       <c r="D39" s="4" t="s">
         <v>140</v>
       </c>
@@ -1800,10 +1800,10 @@
       <c r="B42" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G42" s="13" t="s">
+      <c r="G42" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="H42" s="13"/>
+      <c r="H42" s="11"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="3" t="s">
@@ -1812,10 +1812,10 @@
       <c r="B43" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D43" s="17" t="s">
+      <c r="D43" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E43" s="15"/>
+      <c r="E43" s="13"/>
       <c r="G43" s="3" t="s">
         <v>1</v>
       </c>
@@ -1892,10 +1892,10 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="13" t="s">
+      <c r="A48" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B48" s="13"/>
+      <c r="B48" s="11"/>
       <c r="G48" s="3" t="s">
         <v>35</v>
       </c>
@@ -1910,10 +1910,10 @@
       <c r="B49" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D49" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="E49" s="13"/>
+      <c r="E49" s="11"/>
       <c r="G49" s="3" t="s">
         <v>36</v>
       </c>
@@ -1948,10 +1948,10 @@
       <c r="E51" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G51" s="17" t="s">
+      <c r="G51" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="H51" s="15"/>
+      <c r="H51" s="13"/>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="3" t="s">
@@ -1974,10 +1974,10 @@
       <c r="B53" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D53" s="17" t="s">
+      <c r="D53" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="E53" s="15"/>
+      <c r="E53" s="13"/>
       <c r="G53" s="3" t="s">
         <v>130</v>
       </c>
@@ -2012,10 +2012,10 @@
       <c r="E55" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G55" s="17" t="s">
+      <c r="G55" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="H55" s="15"/>
+      <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" s="3" t="s">
@@ -2078,10 +2078,10 @@
       <c r="B59" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="D59" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="E59" s="15"/>
+      <c r="E59" s="13"/>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="3" t="s">
@@ -2096,14 +2096,14 @@
       <c r="E60" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G60" s="14" t="s">
+      <c r="G60" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="H60" s="15"/>
-      <c r="I60" s="11" t="s">
+      <c r="H60" s="13"/>
+      <c r="I60" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="J60" s="12"/>
+      <c r="J60" s="16"/>
       <c r="K60" s="1"/>
     </row>
     <row r="61" spans="1:11">
@@ -2121,10 +2121,10 @@
       </c>
     </row>
     <row r="62" spans="1:11">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="B62" s="13"/>
+      <c r="B62" s="11"/>
       <c r="D62" s="3" t="s">
         <v>110</v>
       </c>
@@ -2240,10 +2240,10 @@
       </c>
     </row>
     <row r="72" spans="1:10">
-      <c r="A72" s="13" t="s">
+      <c r="A72" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B72" s="13"/>
+      <c r="B72" s="11"/>
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="3" t="s">
@@ -2367,22 +2367,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D15:E15"/>
     <mergeCell ref="I60:J60"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="G1:H1"/>
@@ -2395,6 +2379,22 @@
     <mergeCell ref="G55:H55"/>
     <mergeCell ref="G51:H51"/>
     <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D59:E59"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>